<commit_message>
Change to Article, Padam template corr 08/01/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 3.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 3.5 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5025" uniqueCount="1403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5027" uniqueCount="1402">
   <si>
     <t>PS</t>
   </si>
@@ -4203,9 +4203,6 @@
   </si>
   <si>
     <t>N[s]</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
   <si>
     <t>parA# |</t>
@@ -4388,12 +4385,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -4401,6 +4392,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4432,7 +4429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4598,29 +4595,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4629,13 +4609,7 @@
     <xf numFmtId="49" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4646,16 +4620,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4941,9 +4915,9 @@
   <dimension ref="A1:V2393"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1782" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1784" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1784" sqref="N1784"/>
+      <selection pane="bottomLeft" activeCell="M1791" sqref="A1791:XFD1791"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -7428,7 +7402,7 @@
       <c r="F50" s="20"/>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
-      <c r="I50" s="63" t="s">
+      <c r="I50" s="57" t="s">
         <v>250</v>
       </c>
       <c r="J50" s="5">
@@ -7450,12 +7424,12 @@
         <v>312</v>
       </c>
       <c r="O50" s="7"/>
-      <c r="P50" s="64"/>
-      <c r="Q50" s="64"/>
-      <c r="R50" s="64"/>
-      <c r="S50" s="64"/>
-      <c r="T50" s="64"/>
-      <c r="U50" s="64"/>
+      <c r="P50" s="58"/>
+      <c r="Q50" s="58"/>
+      <c r="R50" s="58"/>
+      <c r="S50" s="58"/>
+      <c r="T50" s="58"/>
+      <c r="U50" s="58"/>
       <c r="V50" s="51"/>
     </row>
     <row r="51" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -7464,7 +7438,7 @@
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
-      <c r="I51" s="63" t="s">
+      <c r="I51" s="57" t="s">
         <v>250</v>
       </c>
       <c r="J51" s="5">
@@ -7486,12 +7460,12 @@
         <v>313</v>
       </c>
       <c r="O51" s="34"/>
-      <c r="P51" s="64"/>
-      <c r="Q51" s="64"/>
-      <c r="R51" s="64"/>
-      <c r="S51" s="64"/>
-      <c r="T51" s="64"/>
-      <c r="U51" s="64"/>
+      <c r="P51" s="58"/>
+      <c r="Q51" s="58"/>
+      <c r="R51" s="58"/>
+      <c r="S51" s="58"/>
+      <c r="T51" s="58"/>
+      <c r="U51" s="58"/>
       <c r="V51" s="51"/>
     </row>
     <row r="52" spans="1:22" s="8" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28059,7 +28033,7 @@
         <v>1291</v>
       </c>
       <c r="T602" s="7" t="s">
-        <v>1322</v>
+        <v>1397</v>
       </c>
       <c r="U602" s="7"/>
       <c r="V602" s="45"/>
@@ -30933,8 +30907,12 @@
       <c r="P679" s="7"/>
       <c r="Q679" s="7"/>
       <c r="R679" s="7"/>
-      <c r="S679" s="7"/>
-      <c r="T679" s="7"/>
+      <c r="S679" s="7" t="s">
+        <v>1270</v>
+      </c>
+      <c r="T679" s="7" t="s">
+        <v>1391</v>
+      </c>
       <c r="U679" s="7"/>
       <c r="V679" s="45"/>
     </row>
@@ -33289,7 +33267,7 @@
       <c r="F745" s="20"/>
       <c r="G745" s="20"/>
       <c r="H745" s="20"/>
-      <c r="I745" s="63" t="s">
+      <c r="I745" s="57" t="s">
         <v>264</v>
       </c>
       <c r="J745" s="9">
@@ -33311,7 +33289,7 @@
         <v>570</v>
       </c>
       <c r="O745" s="34"/>
-      <c r="P745" s="64" t="s">
+      <c r="P745" s="58" t="s">
         <v>18</v>
       </c>
       <c r="Q745" s="7"/>
@@ -41678,9 +41656,7 @@
       <c r="R975" s="7"/>
       <c r="S975" s="7"/>
       <c r="T975" s="7"/>
-      <c r="U975" s="7" t="s">
-        <v>1392</v>
-      </c>
+      <c r="U975" s="7"/>
       <c r="V975" s="45"/>
     </row>
     <row r="976" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43813,8 +43789,8 @@
         <f t="shared" si="50"/>
         <v>8</v>
       </c>
-      <c r="N1034" s="66" t="s">
-        <v>1393</v>
+      <c r="N1034" s="59" t="s">
+        <v>1392</v>
       </c>
       <c r="O1034" s="7" t="s">
         <v>1</v>
@@ -49503,29 +49479,29 @@
       <c r="F1193" s="20"/>
       <c r="G1193" s="20"/>
       <c r="H1193" s="20"/>
-      <c r="I1193" s="52" t="s">
+      <c r="I1193" s="57" t="s">
         <v>273</v>
       </c>
       <c r="J1193" s="9">
         <v>24</v>
       </c>
-      <c r="K1193" s="17">
+      <c r="K1193" s="5">
         <f t="shared" si="54"/>
         <v>1192</v>
       </c>
-      <c r="L1193" s="17">
+      <c r="L1193" s="5">
         <f t="shared" si="55"/>
         <v>67</v>
       </c>
-      <c r="M1193" s="17">
+      <c r="M1193" s="5">
         <f t="shared" si="56"/>
         <v>167</v>
       </c>
-      <c r="N1193" s="45" t="s">
+      <c r="N1193" s="51" t="s">
         <v>762</v>
       </c>
-      <c r="O1193" s="6"/>
-      <c r="P1193" s="11" t="s">
+      <c r="O1193" s="34"/>
+      <c r="P1193" s="58" t="s">
         <v>18</v>
       </c>
       <c r="Q1193" s="7"/>
@@ -49533,7 +49509,7 @@
       <c r="S1193" s="7"/>
       <c r="T1193" s="7"/>
       <c r="U1193" s="7"/>
-      <c r="V1193" s="45" t="s">
+      <c r="V1193" s="51" t="s">
         <v>1356</v>
       </c>
     </row>
@@ -57713,7 +57689,7 @@
       <c r="R1417" s="7"/>
       <c r="S1417" s="7"/>
       <c r="T1417" s="7"/>
-      <c r="U1417" s="67" t="s">
+      <c r="U1417" s="60" t="s">
         <v>1298</v>
       </c>
       <c r="V1417" s="45"/>
@@ -57755,7 +57731,7 @@
         <v>1299</v>
       </c>
       <c r="T1418" s="7" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="U1418" s="7"/>
       <c r="V1418" s="45"/>
@@ -62124,44 +62100,42 @@
       <c r="U1536" s="7"/>
       <c r="V1536" s="45"/>
     </row>
-    <row r="1537" spans="3:22" s="76" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="C1537" s="68"/>
-      <c r="D1537" s="69"/>
-      <c r="E1537" s="70"/>
-      <c r="F1537" s="70"/>
-      <c r="G1537" s="70"/>
-      <c r="H1537" s="70"/>
-      <c r="I1537" s="71" t="s">
+    <row r="1537" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="E1537" s="20"/>
+      <c r="F1537" s="20"/>
+      <c r="G1537" s="20"/>
+      <c r="H1537" s="20"/>
+      <c r="I1537" s="57" t="s">
         <v>280</v>
       </c>
-      <c r="J1537" s="72">
+      <c r="J1537" s="9">
         <v>31</v>
       </c>
-      <c r="K1537" s="73">
+      <c r="K1537" s="5">
         <f t="shared" si="69"/>
         <v>1536</v>
       </c>
-      <c r="L1537" s="73">
+      <c r="L1537" s="5">
         <f t="shared" si="70"/>
         <v>37</v>
       </c>
-      <c r="M1537" s="73">
+      <c r="M1537" s="5">
         <f t="shared" si="71"/>
         <v>137</v>
       </c>
-      <c r="N1537" s="74" t="s">
+      <c r="N1537" s="51" t="s">
         <v>880</v>
       </c>
-      <c r="O1537" s="67"/>
-      <c r="P1537" s="75" t="s">
+      <c r="O1537" s="7"/>
+      <c r="P1537" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="Q1537" s="67"/>
-      <c r="R1537" s="67"/>
-      <c r="S1537" s="67"/>
-      <c r="T1537" s="67"/>
-      <c r="U1537" s="67"/>
-      <c r="V1537" s="74" t="s">
+      <c r="Q1537" s="7"/>
+      <c r="R1537" s="7"/>
+      <c r="S1537" s="7"/>
+      <c r="T1537" s="7"/>
+      <c r="U1537" s="7"/>
+      <c r="V1537" s="51" t="s">
         <v>1362</v>
       </c>
     </row>
@@ -62359,7 +62333,7 @@
       <c r="Q1542" s="7"/>
       <c r="R1542" s="7"/>
       <c r="S1542" s="7" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="T1542" s="7"/>
       <c r="U1542" s="7"/>
@@ -65263,7 +65237,7 @@
         <v>933</v>
       </c>
       <c r="S1627" s="1" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="T1627" s="1" t="s">
         <v>1300</v>
@@ -65321,7 +65295,7 @@
         <v>92</v>
       </c>
       <c r="N1629" s="45" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="O1629" s="7" t="s">
         <v>0</v>
@@ -66203,7 +66177,7 @@
         <v>1291</v>
       </c>
       <c r="T1658" s="1" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="V1658" s="45"/>
     </row>
@@ -67050,10 +67024,10 @@
       </c>
       <c r="O1687" s="7"/>
       <c r="S1687" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="T1687" s="1" t="s">
         <v>1399</v>
-      </c>
-      <c r="T1687" s="1" t="s">
-        <v>1400</v>
       </c>
       <c r="V1687" s="45"/>
     </row>
@@ -67239,7 +67213,7 @@
         <v>18</v>
       </c>
       <c r="U1693" s="1" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="V1693" s="45" t="s">
         <v>1380</v>
@@ -67367,10 +67341,10 @@
       </c>
       <c r="O1697" s="6"/>
       <c r="S1697" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="T1697" s="1" t="s">
         <v>1399</v>
-      </c>
-      <c r="T1697" s="1" t="s">
-        <v>1400</v>
       </c>
       <c r="V1697" s="45"/>
     </row>
@@ -68353,7 +68327,7 @@
       </c>
       <c r="P1730" s="7"/>
       <c r="S1730" s="1" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="V1730" s="45"/>
     </row>
@@ -68835,6 +68809,9 @@
       <c r="N1746" s="45" t="s">
         <v>178</v>
       </c>
+      <c r="U1746" s="1" t="s">
+        <v>1317</v>
+      </c>
       <c r="V1746" s="45"/>
     </row>
     <row r="1747" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69208,7 +69185,7 @@
       </c>
       <c r="O1758" s="6"/>
       <c r="U1758" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="V1758" s="45"/>
     </row>
@@ -70143,46 +70120,46 @@
       </c>
       <c r="V1790" s="45"/>
     </row>
-    <row r="1791" spans="3:22" s="65" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="C1791" s="77" t="s">
+    <row r="1791" spans="3:22" s="67" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1791" s="68" t="s">
         <v>1308</v>
       </c>
-      <c r="D1791" s="58"/>
-      <c r="E1791" s="57"/>
-      <c r="F1791" s="57"/>
-      <c r="G1791" s="57"/>
-      <c r="H1791" s="57"/>
-      <c r="I1791" s="59" t="s">
+      <c r="D1791" s="62"/>
+      <c r="E1791" s="61"/>
+      <c r="F1791" s="61"/>
+      <c r="G1791" s="61"/>
+      <c r="H1791" s="61"/>
+      <c r="I1791" s="63" t="s">
         <v>285</v>
       </c>
-      <c r="J1791" s="78">
+      <c r="J1791" s="69">
         <v>36</v>
       </c>
-      <c r="K1791" s="60">
+      <c r="K1791" s="64">
         <f t="shared" si="81"/>
         <v>1790</v>
       </c>
-      <c r="L1791" s="60">
+      <c r="L1791" s="64">
         <f t="shared" si="82"/>
         <v>54</v>
       </c>
-      <c r="M1791" s="60">
+      <c r="M1791" s="64">
         <f t="shared" si="83"/>
         <v>254</v>
       </c>
-      <c r="N1791" s="61" t="s">
+      <c r="N1791" s="65" t="s">
         <v>1021</v>
       </c>
-      <c r="O1791" s="79"/>
-      <c r="P1791" s="62" t="s">
+      <c r="O1791" s="70"/>
+      <c r="P1791" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="Q1791" s="80"/>
-      <c r="R1791" s="80"/>
-      <c r="S1791" s="80"/>
-      <c r="T1791" s="80"/>
-      <c r="U1791" s="80"/>
-      <c r="V1791" s="61" t="s">
+      <c r="Q1791" s="71"/>
+      <c r="R1791" s="71"/>
+      <c r="S1791" s="71"/>
+      <c r="T1791" s="71"/>
+      <c r="U1791" s="71"/>
+      <c r="V1791" s="65" t="s">
         <v>1388</v>
       </c>
     </row>

</xml_diff>